<commit_message>
Update 08.10 versao lista funcionario
</commit_message>
<xml_diff>
--- a/uploads/ATivosPB.xlsx
+++ b/uploads/ATivosPB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emiteli-my.sharepoint.com/personal/julio_carvalho_emiteli_com_br/Documents/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A207723-D3BF-4FED-AC9D-80BF1AAAC1CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{6A207723-D3BF-4FED-AC9D-80BF1AAAC1CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1023C92A-3A05-4E2F-A4DB-FE2427BAD532}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7BEFB661-3EE2-4317-BE5A-0739F8EA2616}"/>
   </bookViews>
@@ -2253,10 +2253,25 @@
   <dimension ref="A1:M366"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+      <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="47.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>